<commit_message>
redundancies in data  removed
</commit_message>
<xml_diff>
--- a/real3.xlsx
+++ b/real3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TEJAS KHANOLKAR\Desktop\ML fake profile detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA48E75B-EA51-4C05-86DF-51D17C2F55AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E60D97-3174-4787-A7B6-25DF5394A66F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{991C3287-756D-F34B-9FC2-6E987518D8FA}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="206">
   <si>
     <t>caste1</t>
   </si>
@@ -179,9 +179,6 @@
     <t>INR 3 lakhs to 4 lakhs</t>
   </si>
   <si>
-    <t>INR Don't wish to specify</t>
-  </si>
-  <si>
     <t>Health Care</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>Chambhar</t>
   </si>
   <si>
-    <t>INR 50 thousand to  1 lakh</t>
-  </si>
-  <si>
     <t>Construction</t>
   </si>
   <si>
@@ -248,9 +242,6 @@
     <t>INR Under 50 thousand</t>
   </si>
   <si>
-    <t>Himachali</t>
-  </si>
-  <si>
     <t>Mahisya</t>
   </si>
   <si>
@@ -296,9 +287,6 @@
     <t>Kamma</t>
   </si>
   <si>
-    <t>INR 30 lakhs to 35 lakhs</t>
-  </si>
-  <si>
     <t>Kutchi</t>
   </si>
   <si>
@@ -335,9 +323,6 @@
     <t>Kayastha</t>
   </si>
   <si>
-    <t>Unspecified Don't wish to specify</t>
-  </si>
-  <si>
     <t>Loss Prevention Manager</t>
   </si>
   <si>
@@ -416,9 +401,6 @@
     <t>Sikh - Ramgharia</t>
   </si>
   <si>
-    <t>INR 35 lakhs to 40 lakhs</t>
-  </si>
-  <si>
     <t>Sikh</t>
   </si>
   <si>
@@ -611,9 +593,6 @@
     <t>Kurmi Kshatriya</t>
   </si>
   <si>
-    <t>Brahmin - Dixit/Brahmin - Iyer/Brahmin - Pushkarna/Brahmin - Smartha</t>
-  </si>
-  <si>
     <t>Customer Service/Call Centre/BPO</t>
   </si>
   <si>
@@ -660,6 +639,15 @@
   </si>
   <si>
     <t>Civil Services/Law Enforcement</t>
+  </si>
+  <si>
+    <t>Don't wish to specify</t>
+  </si>
+  <si>
+    <t>INR 30 lakhs to 40 lakhs</t>
+  </si>
+  <si>
+    <t>INR 50 thousand to 1 lakh</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FC1675-3D0B-854F-829C-8C36F5C7F113}">
   <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="K21" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1088,7 +1076,7 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -1114,7 +1102,7 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1244,7 +1232,7 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -1310,19 +1298,19 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
@@ -1333,10 +1321,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
         <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -1348,7 +1336,7 @@
         <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G13" t="s">
         <v>40</v>
@@ -1359,10 +1347,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -1371,10 +1359,10 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
@@ -1385,7 +1373,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
         <v>42</v>
@@ -1394,13 +1382,13 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="E15" t="s">
         <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1411,7 +1399,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -1423,7 +1411,7 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
         <v>27</v>
@@ -1437,19 +1425,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
         <v>39</v>
@@ -1463,10 +1451,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1489,10 +1477,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -1504,7 +1492,7 @@
         <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
@@ -1515,19 +1503,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
         <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s">
         <v>39</v>
@@ -1541,7 +1529,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
@@ -1567,7 +1555,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -1579,10 +1567,10 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F22" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
@@ -1593,7 +1581,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
@@ -1602,10 +1590,10 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
@@ -1619,19 +1607,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
@@ -1645,22 +1633,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F25" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
@@ -1671,22 +1659,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="E26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G26" t="s">
         <v>14</v>
@@ -1697,7 +1685,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -1709,10 +1697,10 @@
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G27" t="s">
         <v>14</v>
@@ -1723,25 +1711,25 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
         <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H28" t="s">
         <v>15</v>
@@ -1749,7 +1737,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
         <v>47</v>
@@ -1761,7 +1749,7 @@
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
         <v>27</v>
@@ -1775,10 +1763,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
@@ -1787,10 +1775,10 @@
         <v>18</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G30" t="s">
         <v>14</v>
@@ -1801,22 +1789,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F31" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G31" t="s">
         <v>40</v>
@@ -1827,10 +1815,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
@@ -1839,7 +1827,7 @@
         <v>18</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F32" t="s">
         <v>27</v>
@@ -1853,22 +1841,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F33" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G33" t="s">
         <v>14</v>
@@ -1879,7 +1867,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
@@ -1888,7 +1876,7 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1908,7 +1896,7 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
@@ -1917,10 +1905,10 @@
         <v>18</v>
       </c>
       <c r="E35" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F35" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G35" t="s">
         <v>14</v>
@@ -1931,10 +1919,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>
@@ -1943,10 +1931,10 @@
         <v>26</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G36" t="s">
         <v>14</v>
@@ -1957,7 +1945,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
@@ -1972,7 +1960,7 @@
         <v>32</v>
       </c>
       <c r="F37" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -1986,7 +1974,7 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
@@ -1995,10 +1983,10 @@
         <v>18</v>
       </c>
       <c r="E38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G38" t="s">
         <v>14</v>
@@ -2009,7 +1997,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
         <v>25</v>
@@ -2018,10 +2006,10 @@
         <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E39" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F39" t="s">
         <v>35</v>
@@ -2035,7 +2023,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -2044,13 +2032,13 @@
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F40" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G40" t="s">
         <v>14</v>
@@ -2061,7 +2049,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
@@ -2070,13 +2058,13 @@
         <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="E41" t="s">
         <v>32</v>
       </c>
       <c r="F41" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G41" t="s">
         <v>14</v>
@@ -2087,13 +2075,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -2102,7 +2090,7 @@
         <v>45</v>
       </c>
       <c r="F42" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G42" t="s">
         <v>14</v>
@@ -2113,22 +2101,22 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F43" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G43" t="s">
         <v>14</v>
@@ -2139,7 +2127,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
@@ -2148,13 +2136,13 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G44" t="s">
         <v>14</v>
@@ -2165,13 +2153,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D45" t="s">
         <v>43</v>
@@ -2180,7 +2168,7 @@
         <v>32</v>
       </c>
       <c r="F45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G45" t="s">
         <v>14</v>
@@ -2191,10 +2179,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
         <v>10</v>
@@ -2203,10 +2191,10 @@
         <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F46" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G46" t="s">
         <v>14</v>
@@ -2217,10 +2205,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
@@ -2229,10 +2217,10 @@
         <v>48</v>
       </c>
       <c r="E47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F47" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G47" t="s">
         <v>14</v>
@@ -2243,7 +2231,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
@@ -2255,10 +2243,10 @@
         <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F48" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G48" t="s">
         <v>14</v>
@@ -2269,19 +2257,19 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D49" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F49" t="s">
         <v>35</v>
@@ -2295,25 +2283,25 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D50" t="s">
         <v>18</v>
       </c>
       <c r="E50" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F50" t="s">
         <v>35</v>
       </c>
       <c r="G50" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H50" t="s">
         <v>15</v>
@@ -2321,10 +2309,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
         <v>10</v>
@@ -2336,7 +2324,7 @@
         <v>45</v>
       </c>
       <c r="F51" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G51" t="s">
         <v>14</v>
@@ -2347,22 +2335,22 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D52" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="E52" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F52" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
@@ -2373,19 +2361,19 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D53" t="s">
         <v>31</v>
       </c>
       <c r="E53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F53" t="s">
         <v>33</v>
@@ -2399,10 +2387,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s">
         <v>10</v>
@@ -2414,7 +2402,7 @@
         <v>32</v>
       </c>
       <c r="F54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G54" t="s">
         <v>14</v>
@@ -2425,19 +2413,19 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C55" t="s">
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="E55" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="F55" t="s">
         <v>27</v>
@@ -2451,7 +2439,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
@@ -2463,7 +2451,7 @@
         <v>26</v>
       </c>
       <c r="E56" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F56" t="s">
         <v>35</v>
@@ -2477,22 +2465,22 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C57" t="s">
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="E57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F57" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G57" t="s">
         <v>14</v>
@@ -2515,7 +2503,7 @@
         <v>18</v>
       </c>
       <c r="E58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F58" t="s">
         <v>35</v>
@@ -2529,7 +2517,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B59" t="s">
         <v>29</v>
@@ -2538,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="D59" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="E59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F59" t="s">
         <v>13</v>
@@ -2555,7 +2543,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
         <v>25</v>
@@ -2564,16 +2552,16 @@
         <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E60" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F60" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G60" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H60" t="s">
         <v>15</v>
@@ -2581,10 +2569,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C61" t="s">
         <v>10</v>
@@ -2607,7 +2595,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
@@ -2619,7 +2607,7 @@
         <v>31</v>
       </c>
       <c r="E62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F62" t="s">
         <v>39</v>
@@ -2633,22 +2621,22 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s">
         <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E63" t="s">
         <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G63" t="s">
         <v>14</v>
@@ -2659,13 +2647,13 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C64" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D64" t="s">
         <v>48</v>
@@ -2674,7 +2662,7 @@
         <v>32</v>
       </c>
       <c r="F64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G64" t="s">
         <v>14</v>
@@ -2685,7 +2673,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
@@ -2720,13 +2708,13 @@
         <v>10</v>
       </c>
       <c r="D66" t="s">
+        <v>203</v>
+      </c>
+      <c r="E66" t="s">
+        <v>54</v>
+      </c>
+      <c r="F66" t="s">
         <v>49</v>
-      </c>
-      <c r="E66" t="s">
-        <v>55</v>
-      </c>
-      <c r="F66" t="s">
-        <v>50</v>
       </c>
       <c r="G66" t="s">
         <v>14</v>
@@ -2737,25 +2725,25 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C67" t="s">
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E67" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F67" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G67" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H67" t="s">
         <v>15</v>
@@ -2769,16 +2757,16 @@
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D68" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E68" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F68" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G68" t="s">
         <v>23</v>
@@ -2789,16 +2777,16 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B69" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C69" t="s">
         <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E69" t="s">
         <v>45</v>
@@ -2815,19 +2803,19 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C70" t="s">
         <v>37</v>
       </c>
       <c r="D70" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F70" t="s">
         <v>27</v>
@@ -2841,13 +2829,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C71" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D71" t="s">
         <v>48</v>
@@ -2856,7 +2844,7 @@
         <v>45</v>
       </c>
       <c r="F71" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G71" t="s">
         <v>14</v>
@@ -2867,10 +2855,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B72" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C72" t="s">
         <v>37</v>
@@ -2879,7 +2867,7 @@
         <v>18</v>
       </c>
       <c r="E72" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F72" t="s">
         <v>27</v>
@@ -2893,7 +2881,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B73" t="s">
         <v>9</v>
@@ -2902,16 +2890,16 @@
         <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>128</v>
+        <v>204</v>
       </c>
       <c r="E73" t="s">
         <v>24</v>
       </c>
       <c r="F73" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G73" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H73" t="s">
         <v>15</v>
@@ -2919,7 +2907,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B74" t="s">
         <v>25</v>
@@ -2931,10 +2919,10 @@
         <v>18</v>
       </c>
       <c r="E74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F74" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G74" t="s">
         <v>14</v>
@@ -2945,7 +2933,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B75" t="s">
         <v>29</v>
@@ -2957,10 +2945,10 @@
         <v>18</v>
       </c>
       <c r="E75" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F75" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G75" t="s">
         <v>14</v>
@@ -2971,10 +2959,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B76" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C76" t="s">
         <v>10</v>
@@ -2986,7 +2974,7 @@
         <v>45</v>
       </c>
       <c r="F76" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="G76" t="s">
         <v>14</v>
@@ -2997,7 +2985,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B77" t="s">
         <v>25</v>
@@ -3009,10 +2997,10 @@
         <v>48</v>
       </c>
       <c r="E77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F77" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G77" t="s">
         <v>14</v>
@@ -3023,22 +3011,22 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B78" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C78" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D78" t="s">
         <v>18</v>
       </c>
       <c r="E78" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F78" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G78" t="s">
         <v>14</v>
@@ -3049,13 +3037,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B79" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C79" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D79" t="s">
         <v>31</v>
@@ -3064,7 +3052,7 @@
         <v>32</v>
       </c>
       <c r="F79" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G79" t="s">
         <v>14</v>
@@ -3075,22 +3063,22 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C80" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D80" t="s">
         <v>31</v>
       </c>
       <c r="E80" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F80" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G80" t="s">
         <v>14</v>
@@ -3101,22 +3089,22 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B81" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C81" t="s">
         <v>10</v>
       </c>
       <c r="D81" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E81" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F81" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G81" t="s">
         <v>14</v>
@@ -3127,7 +3115,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B82" t="s">
         <v>29</v>
@@ -3142,7 +3130,7 @@
         <v>45</v>
       </c>
       <c r="F82" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G82" t="s">
         <v>14</v>
@@ -3168,7 +3156,7 @@
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G83" t="s">
         <v>14</v>
@@ -3179,10 +3167,10 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C84" t="s">
         <v>30</v>
@@ -3191,10 +3179,10 @@
         <v>18</v>
       </c>
       <c r="E84" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F84" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G84" t="s">
         <v>14</v>
@@ -3205,22 +3193,22 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B85" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C85" t="s">
         <v>10</v>
       </c>
       <c r="D85" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E85" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F85" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G85" t="s">
         <v>14</v>
@@ -3243,10 +3231,10 @@
         <v>31</v>
       </c>
       <c r="E86" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F86" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G86" t="s">
         <v>23</v>
@@ -3257,22 +3245,22 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B87" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C87" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D87" t="s">
         <v>18</v>
       </c>
       <c r="E87" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F87" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G87" t="s">
         <v>14</v>
@@ -3283,10 +3271,10 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B88" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C88" t="s">
         <v>37</v>
@@ -3295,10 +3283,10 @@
         <v>11</v>
       </c>
       <c r="E88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F88" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G88" t="s">
         <v>23</v>
@@ -3324,7 +3312,7 @@
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G89" t="s">
         <v>14</v>
@@ -3335,7 +3323,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B90" t="s">
         <v>25</v>
@@ -3347,10 +3335,10 @@
         <v>43</v>
       </c>
       <c r="E90" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F90" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G90" t="s">
         <v>40</v>
@@ -3387,22 +3375,22 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B92" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C92" t="s">
         <v>37</v>
       </c>
       <c r="D92" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E92" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F92" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G92" t="s">
         <v>40</v>
@@ -3416,16 +3404,16 @@
         <v>28</v>
       </c>
       <c r="B93" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C93" t="s">
         <v>37</v>
       </c>
       <c r="D93" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E93" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F93" t="s">
         <v>27</v>
@@ -3442,19 +3430,19 @@
         <v>28</v>
       </c>
       <c r="B94" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C94" t="s">
         <v>10</v>
       </c>
       <c r="D94" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E94" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F94" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G94" t="s">
         <v>14</v>
@@ -3465,10 +3453,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B95" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C95" t="s">
         <v>30</v>
@@ -3477,7 +3465,7 @@
         <v>11</v>
       </c>
       <c r="E95" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F95" t="s">
         <v>39</v>
@@ -3503,10 +3491,10 @@
         <v>11</v>
       </c>
       <c r="E96" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F96" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G96" t="s">
         <v>14</v>
@@ -3517,13 +3505,13 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B97" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C97" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D97" t="s">
         <v>18</v>
@@ -3532,7 +3520,7 @@
         <v>45</v>
       </c>
       <c r="F97" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G97" t="s">
         <v>14</v>
@@ -3543,10 +3531,10 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B98" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C98" t="s">
         <v>30</v>
@@ -3555,10 +3543,10 @@
         <v>11</v>
       </c>
       <c r="E98" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F98" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G98" t="s">
         <v>14</v>
@@ -3569,7 +3557,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B99" t="s">
         <v>25</v>
@@ -3584,7 +3572,7 @@
         <v>32</v>
       </c>
       <c r="F99" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G99" t="s">
         <v>14</v>
@@ -3595,10 +3583,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B100" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C100" t="s">
         <v>37</v>
@@ -3607,10 +3595,10 @@
         <v>11</v>
       </c>
       <c r="E100" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F100" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G100" t="s">
         <v>14</v>
@@ -3621,7 +3609,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
@@ -3647,10 +3635,10 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C102" t="s">
         <v>10</v>
@@ -3659,10 +3647,10 @@
         <v>43</v>
       </c>
       <c r="E102" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F102" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G102" t="s">
         <v>14</v>
@@ -3673,7 +3661,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
@@ -3682,10 +3670,10 @@
         <v>37</v>
       </c>
       <c r="D103" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="E103" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F103" t="s">
         <v>13</v>
@@ -3702,7 +3690,7 @@
         <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C104" t="s">
         <v>37</v>
@@ -3711,10 +3699,10 @@
         <v>11</v>
       </c>
       <c r="E104" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="F104" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="G104" t="s">
         <v>14</v>
@@ -3725,19 +3713,19 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B105" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C105" t="s">
         <v>10</v>
       </c>
       <c r="D105" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E105" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F105" t="s">
         <v>27</v>
@@ -3751,19 +3739,19 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B106" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C106" t="s">
         <v>37</v>
       </c>
       <c r="D106" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E106" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F106" t="s">
         <v>27</v>
@@ -3777,22 +3765,22 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B107" t="s">
         <v>25</v>
       </c>
       <c r="C107" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D107" t="s">
         <v>11</v>
       </c>
       <c r="E107" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F107" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G107" t="s">
         <v>14</v>
@@ -3803,7 +3791,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
@@ -3829,7 +3817,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B109" t="s">
         <v>9</v>
@@ -3838,13 +3826,13 @@
         <v>37</v>
       </c>
       <c r="D109" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E109" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F109" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G109" t="s">
         <v>14</v>
@@ -3855,10 +3843,10 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B110" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C110" t="s">
         <v>10</v>
@@ -3867,7 +3855,7 @@
         <v>11</v>
       </c>
       <c r="E110" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F110" t="s">
         <v>27</v>
@@ -3884,7 +3872,7 @@
         <v>8</v>
       </c>
       <c r="B111" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C111" t="s">
         <v>37</v>
@@ -3907,22 +3895,22 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B112" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C112" t="s">
         <v>10</v>
       </c>
       <c r="D112" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E112" t="s">
         <v>24</v>
       </c>
       <c r="F112" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G112" t="s">
         <v>14</v>
@@ -3933,10 +3921,10 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B113" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C113" t="s">
         <v>10</v>
@@ -3945,10 +3933,10 @@
         <v>11</v>
       </c>
       <c r="E113" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F113" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G113" t="s">
         <v>14</v>
@@ -3959,7 +3947,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B114" t="s">
         <v>25</v>
@@ -3971,7 +3959,7 @@
         <v>11</v>
       </c>
       <c r="E114" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F114" t="s">
         <v>39</v>
@@ -3997,10 +3985,10 @@
         <v>11</v>
       </c>
       <c r="E115" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F115" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G115" t="s">
         <v>14</v>
@@ -4011,10 +3999,10 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B116" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C116" t="s">
         <v>10</v>
@@ -4023,10 +4011,10 @@
         <v>48</v>
       </c>
       <c r="E116" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F116" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G116" t="s">
         <v>14</v>
@@ -4037,10 +4025,10 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B117" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C117" t="s">
         <v>37</v>
@@ -4049,10 +4037,10 @@
         <v>11</v>
       </c>
       <c r="E117" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F117" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G117" t="s">
         <v>14</v>
@@ -4063,10 +4051,10 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B118" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C118" t="s">
         <v>30</v>
@@ -4075,7 +4063,7 @@
         <v>48</v>
       </c>
       <c r="E118" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F118" t="s">
         <v>33</v>
@@ -4089,10 +4077,10 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B119" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C119" t="s">
         <v>30</v>
@@ -4115,10 +4103,10 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B120" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C120" t="s">
         <v>37</v>
@@ -4141,10 +4129,10 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B121" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C121" t="s">
         <v>37</v>
@@ -4153,7 +4141,7 @@
         <v>11</v>
       </c>
       <c r="E121" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F121" t="s">
         <v>27</v>
@@ -4167,7 +4155,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B122" t="s">
         <v>25</v>
@@ -4179,10 +4167,10 @@
         <v>11</v>
       </c>
       <c r="E122" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F122" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G122" t="s">
         <v>14</v>
@@ -4193,10 +4181,10 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B123" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C123" t="s">
         <v>10</v>
@@ -4219,13 +4207,13 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B124" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C124" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D124" t="s">
         <v>18</v>
@@ -4234,10 +4222,10 @@
         <v>24</v>
       </c>
       <c r="F124" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G124" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H124" t="s">
         <v>15</v>
@@ -4245,7 +4233,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B125" t="s">
         <v>17</v>
@@ -4257,10 +4245,10 @@
         <v>11</v>
       </c>
       <c r="E125" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F125" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G125" t="s">
         <v>14</v>
@@ -4271,10 +4259,10 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B126" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C126" t="s">
         <v>10</v>
@@ -4283,7 +4271,7 @@
         <v>18</v>
       </c>
       <c r="E126" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F126" t="s">
         <v>27</v>
@@ -4297,10 +4285,10 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B127" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C127" t="s">
         <v>37</v>
@@ -4309,10 +4297,10 @@
         <v>11</v>
       </c>
       <c r="E127" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F127" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G127" t="s">
         <v>14</v>
@@ -4323,19 +4311,19 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B128" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C128" t="s">
         <v>37</v>
       </c>
       <c r="D128" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E128" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F128" t="s">
         <v>27</v>
@@ -4349,7 +4337,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B129" t="s">
         <v>9</v>
@@ -4361,10 +4349,10 @@
         <v>31</v>
       </c>
       <c r="E129" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F129" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G129" t="s">
         <v>14</v>
@@ -4375,19 +4363,19 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B130" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C130" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D130" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E130" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F130" t="s">
         <v>39</v>
@@ -4404,7 +4392,7 @@
         <v>8</v>
       </c>
       <c r="B131" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C131" t="s">
         <v>10</v>
@@ -4416,7 +4404,7 @@
         <v>12</v>
       </c>
       <c r="F131" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G131" t="s">
         <v>14</v>
@@ -4427,10 +4415,10 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B132" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C132" t="s">
         <v>10</v>
@@ -4439,10 +4427,10 @@
         <v>11</v>
       </c>
       <c r="E132" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F132" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G132" t="s">
         <v>14</v>
@@ -4453,22 +4441,22 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B133" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C133" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D133" t="s">
         <v>11</v>
       </c>
       <c r="E133" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F133" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G133" t="s">
         <v>14</v>
@@ -4479,22 +4467,22 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B134" t="s">
         <v>9</v>
       </c>
       <c r="C134" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D134" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E134" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F134" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G134" t="s">
         <v>23</v>
@@ -4505,22 +4493,22 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B135" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C135" t="s">
         <v>10</v>
       </c>
       <c r="D135" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="E135" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F135" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G135" t="s">
         <v>14</v>
@@ -4543,10 +4531,10 @@
         <v>11</v>
       </c>
       <c r="E136" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F136" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G136" t="s">
         <v>14</v>
@@ -4560,7 +4548,7 @@
         <v>20</v>
       </c>
       <c r="B137" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C137" t="s">
         <v>10</v>
@@ -4569,10 +4557,10 @@
         <v>11</v>
       </c>
       <c r="E137" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F137" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G137" t="s">
         <v>23</v>
@@ -4583,7 +4571,7 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B138" t="s">
         <v>47</v>
@@ -4595,10 +4583,10 @@
         <v>48</v>
       </c>
       <c r="E138" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F138" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G138" t="s">
         <v>14</v>
@@ -4609,10 +4597,10 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B139" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C139" t="s">
         <v>10</v>
@@ -4621,7 +4609,7 @@
         <v>11</v>
       </c>
       <c r="E139" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F139" t="s">
         <v>27</v>
@@ -4635,22 +4623,22 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B140" t="s">
         <v>9</v>
       </c>
       <c r="C140" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D140" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E140" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F140" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G140" t="s">
         <v>14</v>
@@ -4661,10 +4649,10 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B141" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C141" t="s">
         <v>10</v>
@@ -4673,10 +4661,10 @@
         <v>11</v>
       </c>
       <c r="E141" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F141" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G141" t="s">
         <v>14</v>
@@ -4687,7 +4675,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B142" t="s">
         <v>9</v>
@@ -4713,10 +4701,10 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B143" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C143" t="s">
         <v>37</v>
@@ -4725,7 +4713,7 @@
         <v>11</v>
       </c>
       <c r="E143" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F143" t="s">
         <v>27</v>
@@ -4739,13 +4727,13 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B144" t="s">
         <v>9</v>
       </c>
       <c r="C144" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D144" t="s">
         <v>11</v>
@@ -4765,10 +4753,10 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B145" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C145" t="s">
         <v>10</v>
@@ -4777,7 +4765,7 @@
         <v>48</v>
       </c>
       <c r="E145" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F145" t="s">
         <v>39</v>
@@ -4791,7 +4779,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B146" t="s">
         <v>17</v>
@@ -4803,10 +4791,10 @@
         <v>31</v>
       </c>
       <c r="E146" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F146" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G146" t="s">
         <v>14</v>
@@ -4817,10 +4805,10 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B147" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C147" t="s">
         <v>37</v>
@@ -4829,7 +4817,7 @@
         <v>11</v>
       </c>
       <c r="E147" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F147" t="s">
         <v>27</v>
@@ -4843,7 +4831,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B148" t="s">
         <v>9</v>
@@ -4858,7 +4846,7 @@
         <v>32</v>
       </c>
       <c r="F148" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="G148" t="s">
         <v>14</v>
@@ -4869,7 +4857,7 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B149" t="s">
         <v>9</v>
@@ -4881,10 +4869,10 @@
         <v>31</v>
       </c>
       <c r="E149" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F149" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G149" t="s">
         <v>14</v>
@@ -4895,22 +4883,22 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B150" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C150" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D150" t="s">
         <v>43</v>
       </c>
       <c r="E150" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F150" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G150" t="s">
         <v>14</v>
@@ -4921,10 +4909,10 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B151" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C151" t="s">
         <v>37</v>
@@ -4933,13 +4921,13 @@
         <v>48</v>
       </c>
       <c r="E151" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F151" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G151" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H151" t="s">
         <v>15</v>
@@ -4950,7 +4938,7 @@
         <v>8</v>
       </c>
       <c r="B152" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C152" t="s">
         <v>37</v>
@@ -4959,10 +4947,10 @@
         <v>11</v>
       </c>
       <c r="E152" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F152" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="G152" t="s">
         <v>14</v>
@@ -4973,10 +4961,10 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B153" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C153" t="s">
         <v>37</v>
@@ -4985,7 +4973,7 @@
         <v>11</v>
       </c>
       <c r="E153" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F153" t="s">
         <v>27</v>
@@ -4999,7 +4987,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B154" t="s">
         <v>25</v>
@@ -5011,7 +4999,7 @@
         <v>31</v>
       </c>
       <c r="E154" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F154" t="s">
         <v>27</v>
@@ -5025,10 +5013,10 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B155" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C155" t="s">
         <v>37</v>
@@ -5037,7 +5025,7 @@
         <v>11</v>
       </c>
       <c r="E155" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F155" t="s">
         <v>27</v>
@@ -5051,7 +5039,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B156" t="s">
         <v>9</v>
@@ -5077,7 +5065,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B157" t="s">
         <v>29</v>
@@ -5089,10 +5077,10 @@
         <v>31</v>
       </c>
       <c r="E157" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F157" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G157" t="s">
         <v>14</v>
@@ -5103,22 +5091,22 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B158" t="s">
         <v>25</v>
       </c>
       <c r="C158" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D158" t="s">
         <v>43</v>
       </c>
       <c r="E158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F158" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G158" t="s">
         <v>14</v>
@@ -5129,10 +5117,10 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B159" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C159" t="s">
         <v>37</v>
@@ -5155,7 +5143,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B160" t="s">
         <v>9</v>
@@ -5167,10 +5155,10 @@
         <v>31</v>
       </c>
       <c r="E160" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F160" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G160" t="s">
         <v>14</v>
@@ -5181,7 +5169,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B161" t="s">
         <v>29</v>
@@ -5199,7 +5187,7 @@
         <v>33</v>
       </c>
       <c r="G161" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H161" t="s">
         <v>15</v>
@@ -5213,16 +5201,16 @@
         <v>25</v>
       </c>
       <c r="C162" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D162" t="s">
         <v>31</v>
       </c>
       <c r="E162" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F162" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G162" t="s">
         <v>23</v>
@@ -5233,22 +5221,22 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B163" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C163" t="s">
         <v>10</v>
       </c>
       <c r="D163" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E163" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F163" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G163" t="s">
         <v>14</v>
@@ -5259,10 +5247,10 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B164" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C164" t="s">
         <v>10</v>
@@ -5271,7 +5259,7 @@
         <v>43</v>
       </c>
       <c r="E164" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F164" t="s">
         <v>27</v>
@@ -5294,13 +5282,13 @@
         <v>10</v>
       </c>
       <c r="D165" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E165" t="s">
         <v>12</v>
       </c>
       <c r="F165" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G165" t="s">
         <v>14</v>
@@ -5311,10 +5299,10 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B166" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C166" t="s">
         <v>10</v>
@@ -5326,7 +5314,7 @@
         <v>19</v>
       </c>
       <c r="F166" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G166" t="s">
         <v>14</v>
@@ -5337,22 +5325,22 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B167" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C167" t="s">
         <v>37</v>
       </c>
       <c r="D167" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="E167" t="s">
         <v>24</v>
       </c>
       <c r="F167" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G167" t="s">
         <v>14</v>
@@ -5363,10 +5351,10 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B168" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C168" t="s">
         <v>10</v>
@@ -5378,7 +5366,7 @@
         <v>32</v>
       </c>
       <c r="F168" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G168" t="s">
         <v>14</v>
@@ -5389,19 +5377,19 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B169" t="s">
+        <v>71</v>
+      </c>
+      <c r="C169" t="s">
         <v>74</v>
-      </c>
-      <c r="C169" t="s">
-        <v>77</v>
       </c>
       <c r="D169" t="s">
         <v>18</v>
       </c>
       <c r="E169" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F169" t="s">
         <v>27</v>
@@ -5427,10 +5415,10 @@
         <v>11</v>
       </c>
       <c r="E170" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F170" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G170" t="s">
         <v>14</v>
@@ -5441,7 +5429,7 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B171" t="s">
         <v>25</v>
@@ -5453,10 +5441,10 @@
         <v>48</v>
       </c>
       <c r="E171" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F171" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G171" t="s">
         <v>14</v>
@@ -5467,19 +5455,19 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B172" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C172" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D172" t="s">
         <v>48</v>
       </c>
       <c r="E172" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F172" t="s">
         <v>35</v>
@@ -5496,19 +5484,19 @@
         <v>8</v>
       </c>
       <c r="B173" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C173" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D173" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E173" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F173" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G173" t="s">
         <v>14</v>
@@ -5519,7 +5507,7 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B174" t="s">
         <v>17</v>
@@ -5531,7 +5519,7 @@
         <v>11</v>
       </c>
       <c r="E174" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F174" t="s">
         <v>27</v>
@@ -5545,7 +5533,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B175" t="s">
         <v>9</v>
@@ -5554,7 +5542,7 @@
         <v>10</v>
       </c>
       <c r="D175" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E175" t="s">
         <v>45</v>
@@ -5571,16 +5559,16 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B176" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C176" t="s">
         <v>10</v>
       </c>
       <c r="D176" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E176" t="s">
         <v>45</v>
@@ -5597,10 +5585,10 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B177" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C177" t="s">
         <v>37</v>
@@ -5609,13 +5597,13 @@
         <v>43</v>
       </c>
       <c r="E177" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F177" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G177" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H177" t="s">
         <v>15</v>
@@ -5623,22 +5611,22 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B178" t="s">
         <v>9</v>
       </c>
       <c r="C178" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D178" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E178" t="s">
         <v>38</v>
       </c>
       <c r="F178" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G178" t="s">
         <v>14</v>
@@ -5649,10 +5637,10 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B179" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C179" t="s">
         <v>37</v>
@@ -5661,7 +5649,7 @@
         <v>11</v>
       </c>
       <c r="E179" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F179" t="s">
         <v>27</v>
@@ -5675,7 +5663,7 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B180" t="s">
         <v>9</v>
@@ -5684,10 +5672,10 @@
         <v>37</v>
       </c>
       <c r="D180" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E180" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F180" t="s">
         <v>27</v>
@@ -5701,10 +5689,10 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C181" t="s">
         <v>10</v>
@@ -5713,7 +5701,7 @@
         <v>11</v>
       </c>
       <c r="E181" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F181" t="s">
         <v>27</v>
@@ -5730,7 +5718,7 @@
         <v>8</v>
       </c>
       <c r="B182" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C182" t="s">
         <v>37</v>
@@ -5753,22 +5741,22 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B183" t="s">
         <v>29</v>
       </c>
       <c r="C183" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D183" t="s">
         <v>11</v>
       </c>
       <c r="E183" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F183" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G183" t="s">
         <v>14</v>
@@ -5779,7 +5767,7 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B184" t="s">
         <v>29</v>
@@ -5797,7 +5785,7 @@
         <v>33</v>
       </c>
       <c r="G184" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H184" t="s">
         <v>15</v>
@@ -5805,10 +5793,10 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B185" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C185" t="s">
         <v>10</v>
@@ -5817,10 +5805,10 @@
         <v>11</v>
       </c>
       <c r="E185" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F185" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G185" t="s">
         <v>14</v>
@@ -5834,7 +5822,7 @@
         <v>8</v>
       </c>
       <c r="B186" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C186" t="s">
         <v>10</v>
@@ -5843,10 +5831,10 @@
         <v>11</v>
       </c>
       <c r="E186" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F186" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G186" t="s">
         <v>14</v>
@@ -5857,10 +5845,10 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B187" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C187" t="s">
         <v>10</v>
@@ -5869,10 +5857,10 @@
         <v>48</v>
       </c>
       <c r="E187" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F187" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G187" t="s">
         <v>14</v>
@@ -5883,16 +5871,16 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B188" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C188" t="s">
         <v>10</v>
       </c>
       <c r="D188" t="s">
-        <v>128</v>
+        <v>204</v>
       </c>
       <c r="E188" t="s">
         <v>24</v>
@@ -5901,7 +5889,7 @@
         <v>13</v>
       </c>
       <c r="G188" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H188" t="s">
         <v>15</v>
@@ -5909,10 +5897,10 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B189" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C189" t="s">
         <v>10</v>
@@ -5921,7 +5909,7 @@
         <v>11</v>
       </c>
       <c r="E189" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F189" t="s">
         <v>27</v>
@@ -5935,10 +5923,10 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B190" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C190" t="s">
         <v>10</v>
@@ -5947,10 +5935,10 @@
         <v>18</v>
       </c>
       <c r="E190" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F190" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G190" t="s">
         <v>14</v>
@@ -5961,10 +5949,10 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B191" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C191" t="s">
         <v>10</v>
@@ -5973,10 +5961,10 @@
         <v>48</v>
       </c>
       <c r="E191" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F191" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G191" t="s">
         <v>14</v>
@@ -5999,7 +5987,7 @@
         <v>31</v>
       </c>
       <c r="E192" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F192" t="s">
         <v>13</v>
@@ -6013,10 +6001,10 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B193" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C193" t="s">
         <v>10</v>
@@ -6025,13 +6013,13 @@
         <v>18</v>
       </c>
       <c r="E193" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F193" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G193" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H193" t="s">
         <v>15</v>
@@ -6039,22 +6027,22 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B194" t="s">
         <v>9</v>
       </c>
       <c r="C194" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D194" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E194" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F194" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="G194" t="s">
         <v>14</v>
@@ -6077,7 +6065,7 @@
         <v>11</v>
       </c>
       <c r="E195" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F195" t="s">
         <v>13</v>
@@ -6091,10 +6079,10 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B196" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C196" t="s">
         <v>10</v>
@@ -6103,7 +6091,7 @@
         <v>31</v>
       </c>
       <c r="E196" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F196" t="s">
         <v>27</v>
@@ -6117,7 +6105,7 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B197" t="s">
         <v>9</v>
@@ -6129,13 +6117,13 @@
         <v>43</v>
       </c>
       <c r="E197" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F197" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G197" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H197" t="s">
         <v>15</v>
@@ -6143,10 +6131,10 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B198" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C198" t="s">
         <v>37</v>
@@ -6155,10 +6143,10 @@
         <v>18</v>
       </c>
       <c r="E198" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F198" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G198" t="s">
         <v>14</v>
@@ -6169,10 +6157,10 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B199" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C199" t="s">
         <v>10</v>
@@ -6184,7 +6172,7 @@
         <v>45</v>
       </c>
       <c r="F199" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G199" t="s">
         <v>14</v>
@@ -6195,10 +6183,10 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B200" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C200" t="s">
         <v>10</v>
@@ -6210,7 +6198,7 @@
         <v>45</v>
       </c>
       <c r="F200" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G200" t="s">
         <v>14</v>
@@ -6221,22 +6209,22 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
+        <v>186</v>
+      </c>
+      <c r="B201" t="s">
+        <v>51</v>
+      </c>
+      <c r="C201" t="s">
+        <v>10</v>
+      </c>
+      <c r="D201" t="s">
+        <v>205</v>
+      </c>
+      <c r="E201" t="s">
+        <v>54</v>
+      </c>
+      <c r="F201" t="s">
         <v>192</v>
-      </c>
-      <c r="B201" t="s">
-        <v>52</v>
-      </c>
-      <c r="C201" t="s">
-        <v>10</v>
-      </c>
-      <c r="D201" t="s">
-        <v>57</v>
-      </c>
-      <c r="E201" t="s">
-        <v>55</v>
-      </c>
-      <c r="F201" t="s">
-        <v>199</v>
       </c>
       <c r="G201" t="s">
         <v>14</v>
@@ -6247,7 +6235,7 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B202" t="s">
         <v>9</v>
@@ -6259,10 +6247,10 @@
         <v>43</v>
       </c>
       <c r="E202" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F202" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G202" t="s">
         <v>14</v>
@@ -6273,19 +6261,19 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B203" t="s">
         <v>29</v>
       </c>
       <c r="C203" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D203" t="s">
         <v>26</v>
       </c>
       <c r="E203" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F203" t="s">
         <v>33</v>
@@ -6299,7 +6287,7 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B204" t="s">
         <v>9</v>
@@ -6311,10 +6299,10 @@
         <v>31</v>
       </c>
       <c r="E204" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F204" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G204" t="s">
         <v>14</v>

</xml_diff>